<commit_message>
Update XLSX file with new test cases
</commit_message>
<xml_diff>
--- a/testCasesSample.xlsx
+++ b/testCasesSample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52F58FA-DD08-4269-BFD5-2CC429517BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D236F3E6-AD3C-9748-917B-77FEEEB6F9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="3570" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4960" yWindow="3580" windowWidth="28800" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCaseTemplate" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -236,6 +236,77 @@
   </si>
   <si>
     <t>No bugs and quick seamless purchase experience with eticket receival</t>
+  </si>
+  <si>
+    <t>ReCaptcha_1</t>
+  </si>
+  <si>
+    <t>ReCaptcha component</t>
+  </si>
+  <si>
+    <t>Verify that the CAPTCHA system prevents automated submissions or botting during the ticket purchasing phase.</t>
+  </si>
+  <si>
+    <t>CAPTCHA integrated on the purchase page</t>
+  </si>
+  <si>
+    <t>1. Navigate to the ticket purchase page.
+2. Complete the CAPTCHA challenge incorrectly.
+3. Attempt to submit the purchase form.</t>
+  </si>
+  <si>
+    <t>CAPTCHA challenge must display an error message of failure when completed incorrectly. An error message" ("CAPTCHA validation failed" is shown.</t>
+  </si>
+  <si>
+    <t>Error message "CAPTCHA validation failed" was displayed and the form was blocked.</t>
+  </si>
+  <si>
+    <t>Carlyne</t>
+  </si>
+  <si>
+    <t>AdminPage_1</t>
+  </si>
+  <si>
+    <t>Admin Page</t>
+  </si>
+  <si>
+    <t>Verify that the administrator can access all system data and perform actions on the page.</t>
+  </si>
+  <si>
+    <t>Admin credentials are available.</t>
+  </si>
+  <si>
+    <t>1. Log in using valid administrator credentials.
+2. Navigate to the admin page.
+3. Verify that all data (tickets, feedback, etc.) is displayed without filters.</t>
+  </si>
+  <si>
+    <t>Admin page should display system data with full access to required modifiers and data.</t>
+  </si>
+  <si>
+    <t>Admin login succeeded and all system data would be correctly displayed without filters that are shown with normal users.</t>
+  </si>
+  <si>
+    <t>SessionTimeout_1</t>
+  </si>
+  <si>
+    <t>Session Management</t>
+  </si>
+  <si>
+    <t>Verify that a user is automatically logged out after 10 minutes of inactivity.</t>
+  </si>
+  <si>
+    <t>User is signed in and has an active session running.</t>
+  </si>
+  <si>
+    <t>1. Sign in and remain inactive for over 10 minutes.
+2. Attempt any interaction (ex: navigating to another page).</t>
+  </si>
+  <si>
+    <t>The system should terminate the session and prompt the user to relog with a "Session timed out" notice.</t>
+  </si>
+  <si>
+    <t>The system terminated the session after 10 minutes of inactivity and redirected the user to the login page with a timeout message.</t>
   </si>
 </sst>
 </file>
@@ -644,25 +715,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -676,7 +747,7 @@
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -740,7 +811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
@@ -772,7 +843,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -804,7 +875,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -836,7 +907,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -868,7 +939,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
@@ -900,7 +971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>58</v>
       </c>
@@ -932,7 +1003,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
@@ -964,41 +1035,101 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="2"/>
+    <row r="11" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated testCasesSample.xlsx with new test cases
</commit_message>
<xml_diff>
--- a/testCasesSample.xlsx
+++ b/testCasesSample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D236F3E6-AD3C-9748-917B-77FEEEB6F9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7D633E-9009-0045-965F-8F192EE63023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4960" yWindow="3580" windowWidth="28800" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="89">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Test Executed By</t>
-  </si>
-  <si>
-    <t>Test Case Template</t>
   </si>
   <si>
     <t>Pre-requisites</t>
@@ -77,9 +74,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>TesterK</t>
   </si>
   <si>
     <t>Ticket DB</t>
@@ -307,6 +301,9 @@
   </si>
   <si>
     <t>The system terminated the session after 10 minutes of inactivity and redirected the user to the login page with a timeout message.</t>
+  </si>
+  <si>
+    <t>Test Case San Diego Ticketing System</t>
   </si>
 </sst>
 </file>
@@ -716,7 +713,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -735,7 +732,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -761,7 +758,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
@@ -781,354 +778,354 @@
     </row>
     <row r="3" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="G4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="F5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="G6" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="I8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="H10" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="I11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="I12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="I13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>